<commit_message>
test chuc nang on het roii
</commit_message>
<xml_diff>
--- a/form_collectdata/form_collect/DataCollected/TongHopDiem1.xlsx
+++ b/form_collectdata/form_collect/DataCollected/TongHopDiem1.xlsx
@@ -58,9 +58,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -69,23 +69,26 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -452,7 +455,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AZ8"/>
+  <dimension ref="A1:AZ5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,58 +463,58 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="19.005" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="20.29071428571428" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
-    <col width="16.86214285714286" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
-    <col width="10.71928571428571" bestFit="1" customWidth="1" style="8" min="4" max="4"/>
-    <col width="11.57642857142857" bestFit="1" customWidth="1" style="8" min="5" max="5"/>
-    <col width="10.43357142857143" bestFit="1" customWidth="1" style="8" min="6" max="6"/>
-    <col width="12.14785714285714" bestFit="1" customWidth="1" style="8" min="7" max="7"/>
-    <col width="13.005" bestFit="1" customWidth="1" style="8" min="8" max="8"/>
-    <col width="13.29071428571429" bestFit="1" customWidth="1" style="8" min="9" max="9"/>
-    <col width="11.57642857142857" bestFit="1" customWidth="1" style="8" min="10" max="10"/>
-    <col width="12.29071428571429" bestFit="1" customWidth="1" style="8" min="11" max="11"/>
-    <col width="18.005" bestFit="1" customWidth="1" style="8" min="12" max="12"/>
-    <col width="13.86214285714286" bestFit="1" customWidth="1" style="8" min="13" max="13"/>
-    <col width="12.14785714285714" bestFit="1" customWidth="1" style="8" min="14" max="14"/>
-    <col width="12.005" bestFit="1" customWidth="1" style="8" min="15" max="15"/>
-    <col width="13.29071428571429" bestFit="1" customWidth="1" style="8" min="16" max="16"/>
-    <col width="12.29071428571429" bestFit="1" customWidth="1" style="8" min="17" max="17"/>
-    <col width="11.57642857142857" bestFit="1" customWidth="1" style="8" min="18" max="18"/>
-    <col width="11.57642857142857" bestFit="1" customWidth="1" style="8" min="19" max="19"/>
-    <col width="11.71928571428571" bestFit="1" customWidth="1" style="8" min="20" max="20"/>
-    <col width="9.147857142857141" bestFit="1" customWidth="1" style="8" min="21" max="21"/>
-    <col width="10.71928571428571" bestFit="1" customWidth="1" style="8" min="22" max="22"/>
-    <col width="10.29071428571429" bestFit="1" customWidth="1" style="8" min="23" max="23"/>
-    <col width="10.29071428571429" bestFit="1" customWidth="1" style="8" min="24" max="24"/>
-    <col width="10.29071428571429" bestFit="1" customWidth="1" style="8" min="25" max="25"/>
-    <col width="8.862142857142858" bestFit="1" customWidth="1" style="8" min="26" max="26"/>
-    <col width="8.862142857142858" bestFit="1" customWidth="1" style="8" min="27" max="27"/>
-    <col width="8.862142857142858" bestFit="1" customWidth="1" style="8" min="28" max="28"/>
-    <col width="8.862142857142858" bestFit="1" customWidth="1" style="8" min="29" max="29"/>
-    <col width="8.862142857142858" bestFit="1" customWidth="1" style="8" min="30" max="30"/>
-    <col width="8.862142857142858" bestFit="1" customWidth="1" style="8" min="31" max="31"/>
-    <col width="8.862142857142858" bestFit="1" customWidth="1" style="8" min="32" max="32"/>
-    <col width="14.29071428571429" bestFit="1" customWidth="1" style="8" min="33" max="33"/>
-    <col width="14.29071428571429" bestFit="1" customWidth="1" style="8" min="34" max="34"/>
-    <col width="14.29071428571429" bestFit="1" customWidth="1" style="8" min="35" max="35"/>
-    <col width="14.29071428571429" bestFit="1" customWidth="1" style="8" min="36" max="36"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="37" max="37"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="38" max="38"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="39" max="39"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="40" max="40"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="41" max="41"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="42" max="42"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="43" max="43"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="44" max="44"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="45" max="45"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="46" max="46"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="47" max="47"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="48" max="48"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="49" max="49"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="50" max="50"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="51" max="51"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="52" max="52"/>
+    <col width="19.005" bestFit="1" customWidth="1" style="8" min="1" max="1"/>
+    <col width="20.29071428571428" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="16.86214285714286" bestFit="1" customWidth="1" style="8" min="3" max="3"/>
+    <col width="10.71928571428571" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
+    <col width="11.57642857142857" bestFit="1" customWidth="1" style="9" min="5" max="5"/>
+    <col width="10.43357142857143" bestFit="1" customWidth="1" style="9" min="6" max="6"/>
+    <col width="12.14785714285714" bestFit="1" customWidth="1" style="9" min="7" max="7"/>
+    <col width="13.005" bestFit="1" customWidth="1" style="9" min="8" max="8"/>
+    <col width="13.29071428571429" bestFit="1" customWidth="1" style="9" min="9" max="9"/>
+    <col width="11.57642857142857" bestFit="1" customWidth="1" style="9" min="10" max="10"/>
+    <col width="12.29071428571429" bestFit="1" customWidth="1" style="9" min="11" max="11"/>
+    <col width="18.005" bestFit="1" customWidth="1" style="9" min="12" max="12"/>
+    <col width="13.86214285714286" bestFit="1" customWidth="1" style="9" min="13" max="13"/>
+    <col width="12.14785714285714" bestFit="1" customWidth="1" style="9" min="14" max="14"/>
+    <col width="12.005" bestFit="1" customWidth="1" style="9" min="15" max="15"/>
+    <col width="13.29071428571429" bestFit="1" customWidth="1" style="9" min="16" max="16"/>
+    <col width="12.29071428571429" bestFit="1" customWidth="1" style="9" min="17" max="17"/>
+    <col width="11.57642857142857" bestFit="1" customWidth="1" style="9" min="18" max="18"/>
+    <col width="11.57642857142857" bestFit="1" customWidth="1" style="9" min="19" max="19"/>
+    <col width="11.71928571428571" bestFit="1" customWidth="1" style="9" min="20" max="20"/>
+    <col width="9.147857142857141" bestFit="1" customWidth="1" style="9" min="21" max="21"/>
+    <col width="10.71928571428571" bestFit="1" customWidth="1" style="9" min="22" max="22"/>
+    <col width="10.29071428571429" bestFit="1" customWidth="1" style="9" min="23" max="23"/>
+    <col width="10.29071428571429" bestFit="1" customWidth="1" style="9" min="24" max="24"/>
+    <col width="10.29071428571429" bestFit="1" customWidth="1" style="9" min="25" max="25"/>
+    <col width="8.862142857142858" bestFit="1" customWidth="1" style="9" min="26" max="26"/>
+    <col width="8.862142857142858" bestFit="1" customWidth="1" style="9" min="27" max="27"/>
+    <col width="8.862142857142858" bestFit="1" customWidth="1" style="9" min="28" max="28"/>
+    <col width="8.862142857142858" bestFit="1" customWidth="1" style="9" min="29" max="29"/>
+    <col width="8.862142857142858" bestFit="1" customWidth="1" style="9" min="30" max="30"/>
+    <col width="8.862142857142858" bestFit="1" customWidth="1" style="9" min="31" max="31"/>
+    <col width="8.862142857142858" bestFit="1" customWidth="1" style="9" min="32" max="32"/>
+    <col width="14.29071428571429" bestFit="1" customWidth="1" style="9" min="33" max="33"/>
+    <col width="14.29071428571429" bestFit="1" customWidth="1" style="9" min="34" max="34"/>
+    <col width="14.29071428571429" bestFit="1" customWidth="1" style="9" min="35" max="35"/>
+    <col width="14.29071428571429" bestFit="1" customWidth="1" style="9" min="36" max="36"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="37" max="37"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="38" max="38"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="39" max="39"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="40" max="40"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="41" max="41"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="42" max="42"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="43" max="43"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="44" max="44"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="45" max="45"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="46" max="46"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="47" max="47"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="48" max="48"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="49" max="49"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="50" max="50"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="51" max="51"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="52" max="52"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -545,20 +548,20 @@
           <t>Điểm trung bình CLO</t>
         </is>
       </c>
-      <c r="AQ1" s="4" t="inlineStr">
+      <c r="AQ1" s="5" t="inlineStr">
         <is>
           <t>GPA</t>
         </is>
       </c>
-      <c r="AR1" s="5" t="n"/>
-      <c r="AS1" s="5" t="n"/>
-      <c r="AT1" s="5" t="n"/>
-      <c r="AU1" s="5" t="n"/>
-      <c r="AV1" s="5" t="n"/>
-      <c r="AW1" s="5" t="n"/>
-      <c r="AX1" s="5" t="n"/>
-      <c r="AY1" s="5" t="n"/>
-      <c r="AZ1" s="5" t="n"/>
+      <c r="AR1" s="6" t="n"/>
+      <c r="AS1" s="6" t="n"/>
+      <c r="AT1" s="6" t="n"/>
+      <c r="AU1" s="6" t="n"/>
+      <c r="AV1" s="6" t="n"/>
+      <c r="AW1" s="6" t="n"/>
+      <c r="AX1" s="6" t="n"/>
+      <c r="AY1" s="6" t="n"/>
+      <c r="AZ1" s="6" t="n"/>
     </row>
     <row r="2" ht="19.5" customHeight="1">
       <c r="D2" s="2" t="inlineStr">
@@ -606,45 +609,45 @@
           <t>PB</t>
         </is>
       </c>
-      <c r="AK2" s="4" t="inlineStr">
+      <c r="AK2" s="1" t="inlineStr">
         <is>
           <t>O1</t>
         </is>
       </c>
-      <c r="AL2" s="4" t="inlineStr">
+      <c r="AL2" s="1" t="inlineStr">
         <is>
           <t>O2</t>
         </is>
       </c>
-      <c r="AM2" s="4" t="inlineStr">
+      <c r="AM2" s="5" t="inlineStr">
         <is>
           <t>O3</t>
         </is>
       </c>
-      <c r="AN2" s="4" t="inlineStr">
+      <c r="AN2" s="1" t="inlineStr">
         <is>
           <t>O4</t>
         </is>
       </c>
-      <c r="AO2" s="4" t="inlineStr">
+      <c r="AO2" s="5" t="inlineStr">
         <is>
           <t>O5</t>
         </is>
       </c>
-      <c r="AP2" s="4" t="inlineStr">
+      <c r="AP2" s="1" t="inlineStr">
         <is>
           <t>O6</t>
         </is>
       </c>
-      <c r="AR2" s="5" t="n"/>
-      <c r="AS2" s="5" t="n"/>
-      <c r="AT2" s="5" t="n"/>
-      <c r="AU2" s="5" t="n"/>
-      <c r="AV2" s="5" t="n"/>
-      <c r="AW2" s="5" t="n"/>
-      <c r="AX2" s="5" t="n"/>
-      <c r="AY2" s="5" t="n"/>
-      <c r="AZ2" s="5" t="n"/>
+      <c r="AR2" s="6" t="n"/>
+      <c r="AS2" s="6" t="n"/>
+      <c r="AT2" s="6" t="n"/>
+      <c r="AU2" s="6" t="n"/>
+      <c r="AV2" s="6" t="n"/>
+      <c r="AW2" s="6" t="n"/>
+      <c r="AX2" s="6" t="n"/>
+      <c r="AY2" s="6" t="n"/>
+      <c r="AZ2" s="6" t="n"/>
     </row>
     <row r="3" ht="19.5" customHeight="1">
       <c r="D3" s="2" t="inlineStr">
@@ -812,97 +815,97 @@
           <t>O6</t>
         </is>
       </c>
-      <c r="AR3" s="5" t="n"/>
-      <c r="AS3" s="5" t="n"/>
-      <c r="AT3" s="5" t="n"/>
-      <c r="AU3" s="5" t="n"/>
-      <c r="AV3" s="5" t="n"/>
-      <c r="AW3" s="5" t="n"/>
-      <c r="AX3" s="5" t="n"/>
-      <c r="AY3" s="5" t="n"/>
-      <c r="AZ3" s="5" t="n"/>
+      <c r="AR3" s="6" t="n"/>
+      <c r="AS3" s="6" t="n"/>
+      <c r="AT3" s="6" t="n"/>
+      <c r="AU3" s="6" t="n"/>
+      <c r="AV3" s="6" t="n"/>
+      <c r="AW3" s="6" t="n"/>
+      <c r="AX3" s="6" t="n"/>
+      <c r="AY3" s="6" t="n"/>
+      <c r="AZ3" s="6" t="n"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>La Thị Hồng Nhung</t>
+          <t>Hoàng Tuấn Anh</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>B20DCDT158</t>
+          <t>B20DCDT010</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>D20XLTH</t>
+          <t>D20DTMT1</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X4" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Y4" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Z4" t="n">
         <v>8</v>
@@ -914,132 +917,132 @@
         <v>8</v>
       </c>
       <c r="AC4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AD4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AE4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AF4" t="n">
-        <v>9.5</v>
+        <v>8</v>
       </c>
       <c r="AG4" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AH4" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AI4" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AJ4" t="n">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="AK4" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AL4" t="n">
-        <v>8</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="AM4" t="n">
-        <v>6.75</v>
+        <v>2</v>
       </c>
       <c r="AN4" t="n">
-        <v>6.428571428571429</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="AO4" t="n">
-        <v>6.285714285714286</v>
+        <v>2.285714285714286</v>
       </c>
       <c r="AP4" t="n">
-        <v>6.571428571428571</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="AQ4" t="n">
-        <v>6.839285714285714</v>
+        <v>3.317460317460317</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nguyễn Trung Tuấn</t>
+          <t>Lê Tiến Phát</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>B20DCDT190</t>
+          <t>B20DCDT159</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>D20XLTH</t>
+          <t>D20DTRB</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y5" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Z5" t="n">
         <v>0</v>
@@ -1075,436 +1078,25 @@
         <v>0</v>
       </c>
       <c r="AK5" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AL5" t="n">
         <v>0</v>
       </c>
       <c r="AM5" t="n">
-        <v>3.625</v>
+        <v>0</v>
       </c>
       <c r="AN5" t="n">
-        <v>4.142857142857143</v>
+        <v>0</v>
       </c>
       <c r="AO5" t="n">
-        <v>4.142857142857143</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="AP5" t="n">
-        <v>4.142857142857143</v>
+        <v>0</v>
       </c>
       <c r="AQ5" t="n">
-        <v>2.675595238095239</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Phạm Thế Anh</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>B20DCDT017</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>D20DTMT1</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>3</v>
-      </c>
-      <c r="E6" t="n">
-        <v>3</v>
-      </c>
-      <c r="F6" t="n">
-        <v>3</v>
-      </c>
-      <c r="G6" t="n">
-        <v>3</v>
-      </c>
-      <c r="H6" t="n">
-        <v>4</v>
-      </c>
-      <c r="I6" t="n">
-        <v>4</v>
-      </c>
-      <c r="J6" t="n">
-        <v>4</v>
-      </c>
-      <c r="K6" t="n">
-        <v>4</v>
-      </c>
-      <c r="L6" t="n">
-        <v>5</v>
-      </c>
-      <c r="M6" t="n">
-        <v>5</v>
-      </c>
-      <c r="N6" t="n">
-        <v>5</v>
-      </c>
-      <c r="O6" t="n">
-        <v>5</v>
-      </c>
-      <c r="P6" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>6</v>
-      </c>
-      <c r="R6" t="n">
-        <v>6</v>
-      </c>
-      <c r="S6" t="n">
-        <v>6</v>
-      </c>
-      <c r="T6" t="n">
-        <v>7</v>
-      </c>
-      <c r="U6" t="n">
-        <v>7</v>
-      </c>
-      <c r="V6" t="n">
-        <v>7</v>
-      </c>
-      <c r="W6" t="n">
-        <v>7</v>
-      </c>
-      <c r="X6" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>2</v>
-      </c>
-      <c r="AH6" t="n">
-        <v>2</v>
-      </c>
-      <c r="AI6" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>2</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="AM6" t="n">
-        <v>3.375</v>
-      </c>
-      <c r="AN6" t="n">
-        <v>3.857142857142857</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>3.714285714285714</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>3.857142857142857</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>2.745039682539682</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Nguyễn Tiến Duy</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>B20DCDT037</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>D20DTMT1</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" t="n">
-        <v>3</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3</v>
-      </c>
-      <c r="G7" t="n">
-        <v>3</v>
-      </c>
-      <c r="H7" t="n">
-        <v>4</v>
-      </c>
-      <c r="I7" t="n">
-        <v>4</v>
-      </c>
-      <c r="J7" t="n">
-        <v>4</v>
-      </c>
-      <c r="K7" t="n">
-        <v>4</v>
-      </c>
-      <c r="L7" t="n">
-        <v>5</v>
-      </c>
-      <c r="M7" t="n">
-        <v>5</v>
-      </c>
-      <c r="N7" t="n">
-        <v>5</v>
-      </c>
-      <c r="O7" t="n">
-        <v>5</v>
-      </c>
-      <c r="P7" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>6</v>
-      </c>
-      <c r="R7" t="n">
-        <v>6</v>
-      </c>
-      <c r="S7" t="n">
-        <v>6</v>
-      </c>
-      <c r="T7" t="n">
-        <v>7</v>
-      </c>
-      <c r="U7" t="n">
-        <v>7</v>
-      </c>
-      <c r="V7" t="n">
-        <v>7</v>
-      </c>
-      <c r="W7" t="n">
-        <v>7</v>
-      </c>
-      <c r="X7" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y7" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM7" t="n">
-        <v>3.125</v>
-      </c>
-      <c r="AN7" t="n">
-        <v>3.571428571428572</v>
-      </c>
-      <c r="AO7" t="n">
-        <v>3.571428571428572</v>
-      </c>
-      <c r="AP7" t="n">
-        <v>3.571428571428572</v>
-      </c>
-      <c r="AQ7" t="n">
-        <v>2.306547619047619</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Lê Sỹ Sang</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>B20DCDT175</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>D20DTMT2</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>3</v>
-      </c>
-      <c r="E8" t="n">
-        <v>3</v>
-      </c>
-      <c r="F8" t="n">
-        <v>3</v>
-      </c>
-      <c r="G8" t="n">
-        <v>3</v>
-      </c>
-      <c r="H8" t="n">
-        <v>4</v>
-      </c>
-      <c r="I8" t="n">
-        <v>4</v>
-      </c>
-      <c r="J8" t="n">
-        <v>4</v>
-      </c>
-      <c r="K8" t="n">
-        <v>4</v>
-      </c>
-      <c r="L8" t="n">
-        <v>5</v>
-      </c>
-      <c r="M8" t="n">
-        <v>5</v>
-      </c>
-      <c r="N8" t="n">
-        <v>5</v>
-      </c>
-      <c r="O8" t="n">
-        <v>5</v>
-      </c>
-      <c r="P8" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>6</v>
-      </c>
-      <c r="R8" t="n">
-        <v>6</v>
-      </c>
-      <c r="S8" t="n">
-        <v>6</v>
-      </c>
-      <c r="T8" t="n">
-        <v>7</v>
-      </c>
-      <c r="U8" t="n">
-        <v>7</v>
-      </c>
-      <c r="V8" t="n">
-        <v>7</v>
-      </c>
-      <c r="W8" t="n">
-        <v>7</v>
-      </c>
-      <c r="X8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM8" t="n">
-        <v>3.125</v>
-      </c>
-      <c r="AN8" t="n">
-        <v>3.571428571428572</v>
-      </c>
-      <c r="AO8" t="n">
-        <v>3.571428571428572</v>
-      </c>
-      <c r="AP8" t="n">
-        <v>3.571428571428572</v>
-      </c>
-      <c r="AQ8" t="n">
-        <v>2.306547619047619</v>
+        <v>1.523809523809524</v>
       </c>
     </row>
   </sheetData>

</xml_diff>